<commit_message>
Add FCNN model and dataset classes
</commit_message>
<xml_diff>
--- a/data/original/Nombre de los productos.xlsx
+++ b/data/original/Nombre de los productos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
   <si>
     <t xml:space="preserve">Cell Metrics</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Nocodazol</t>
   </si>
   <si>
-    <t xml:space="preserve">etoposido</t>
+    <t xml:space="preserve">Etoposido</t>
   </si>
   <si>
     <t xml:space="preserve">Tamoxifeno</t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Doxorubicina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Etoposido</t>
   </si>
   <si>
     <t xml:space="preserve">OLL461</t>
@@ -213,10 +210,10 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="2" width="12.43"/>
@@ -349,7 +346,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
@@ -420,10 +417,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -452,13 +449,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -469,13 +466,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>